<commit_message>
removing and saving applied
</commit_message>
<xml_diff>
--- a/_self/_finance/_offering.xlsx
+++ b/_self/_finance/_offering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_git\_spirit\_spiritual_work\_self\_finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trieu/Documents/gitWork/_docs_sources/_self/_finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3CE01C-944C-4099-82D0-FB7BA78D7FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FE4924-6E72-5341-AF30-F4E9844058E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanForMoney" sheetId="2" r:id="rId1"/>
@@ -24,12 +24,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>OFFERING MANAGEMENT FOR SELF</t>
   </si>
@@ -78,9 +74,6 @@
     <t>Tournament</t>
   </si>
   <si>
-    <t>C.Xuân, Khánh Vân (GĐ), Ksor Nhi</t>
-  </si>
-  <si>
     <t>Tháng 10,11,12</t>
   </si>
   <si>
@@ -124,6 +117,18 @@
   </si>
   <si>
     <t>April</t>
+  </si>
+  <si>
+    <t>Nhi + Hoàng</t>
+  </si>
+  <si>
+    <t>Offer as Couple</t>
+  </si>
+  <si>
+    <t>Triệu (600k), c.Diệp (700k - pending), Thới (300)</t>
+  </si>
+  <si>
+    <t>C.Xuân (500k), Khánh Vân (GĐ - (500k)), Ksor Nhi (500k)</t>
   </si>
 </sst>
 </file>
@@ -276,18 +281,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -303,16 +296,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -597,345 +602,329 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E0B97F-FCA8-4FB7-BFBD-FBC6FB241C81}">
   <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="10"/>
-    <col min="2" max="2" width="14.109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" style="10" customWidth="1"/>
-    <col min="6" max="8" width="15.44140625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="10"/>
+    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="2" max="2" width="14.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="15.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="2:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="2:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>15000000</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="12" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="13">
-        <v>15000000</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12" t="s">
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="13">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
         <v>0</v>
       </c>
-      <c r="G7" s="13">
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
         <v>0</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13">
-        <v>3000000</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="H10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13">
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
         <v>0</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13">
-        <v>1500000</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="H11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13">
-        <v>1500000</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13">
-        <v>0</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
-      <c r="C11" s="18">
-        <v>5000000</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13">
-        <v>0</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="13">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="9">
         <f>SUM(B7:B22)</f>
         <v>15000000</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="9">
         <f>SUM(C7:C22)</f>
-        <v>11000000</v>
-      </c>
-      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
         <f>B23-C23</f>
-        <v>4000000</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="13">
+        <v>15000000</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="9">
         <f>SUM(F7:F22)</f>
         <v>0</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="9">
         <f>SUM(G7:G22)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="9">
         <f>F23-G23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="11"/>
+      <c r="F24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="14" t="s">
+      <c r="H24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -952,106 +941,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="143" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="1"/>
-    <col min="2" max="4" width="16.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="1" customWidth="1"/>
     <col min="7" max="8" width="11.6640625" style="1"/>
-    <col min="9" max="13" width="15.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="11.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="I2" s="9" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="I2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+    </row>
+    <row r="5" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -1059,13 +1053,13 @@
         <v>44604</v>
       </c>
       <c r="D7" s="3">
-        <v>1400000</v>
+        <v>1500000</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -1083,11 +1077,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
+    <row r="8" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45048</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1600000</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="I8" s="2">
         <v>2</v>
@@ -1105,31 +1107,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="2">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
+        <v>45046</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
@@ -1141,7 +1155,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
@@ -1153,7 +1167,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
@@ -1165,7 +1179,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
@@ -1177,7 +1191,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
@@ -1189,7 +1203,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
@@ -1201,7 +1215,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
@@ -1213,7 +1227,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
@@ -1225,7 +1239,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
@@ -1237,7 +1251,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
@@ -1249,7 +1263,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="2:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>

</xml_diff>

<commit_message>
Update Files and Information
</commit_message>
<xml_diff>
--- a/_self/_finance/_offering.xlsx
+++ b/_self/_finance/_offering.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trieu/Documents/gitWork/_docs_sources/_self/_finance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trieupn/Documents/work_spaces/serving_self/_docs_sources/_self/_finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C291F2C4-15A2-0446-958E-3D8F03E5441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C59D37-F2A7-EB43-8C27-262E0EACB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PlanForMoney" sheetId="2" r:id="rId1"/>
-    <sheet name="Offering" sheetId="1" r:id="rId2"/>
+    <sheet name="Offering" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,8 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>OFFERING MANAGEMENT FOR SELF</t>
   </si>
@@ -77,48 +79,6 @@
     <t>Tháng 10,11,12</t>
   </si>
   <si>
-    <t>Finance Planning</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Outcome</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Monthly Income</t>
-  </si>
-  <si>
-    <t>For Family</t>
-  </si>
-  <si>
-    <t>Rent Fee</t>
-  </si>
-  <si>
-    <t>Offering 1/10</t>
-  </si>
-  <si>
-    <t>For Saving</t>
-  </si>
-  <si>
-    <t>Total Income</t>
-  </si>
-  <si>
-    <t>Leftover</t>
-  </si>
-  <si>
-    <t>Total Outcome</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
     <t>Nhi + Hoàng</t>
   </si>
   <si>
@@ -129,6 +89,15 @@
   </si>
   <si>
     <t>Triệu (600k), c.Diệp (700k), Thới (300)</t>
+  </si>
+  <si>
+    <t>../07/2023</t>
+  </si>
+  <si>
+    <t>India Mission Trip</t>
+  </si>
+  <si>
+    <t>Thu Hà</t>
   </si>
 </sst>
 </file>
@@ -138,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$VND]\ #,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,27 +128,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="30"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,18 +148,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -264,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,33 +217,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -599,350 +510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E0B97F-FCA8-4FB7-BFBD-FBC6FB241C81}">
-  <dimension ref="B2:I25"/>
-  <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.83203125" style="6"/>
-    <col min="2" max="2" width="14.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="15.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="2:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="2:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="9">
-        <v>15000000</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="9">
-        <f>SUM(B7:B22)</f>
-        <v>15000000</v>
-      </c>
-      <c r="C23" s="9">
-        <f>SUM(C7:C22)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <f>B23-C23</f>
-        <v>15000000</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="9">
-        <f>SUM(F7:F22)</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="9">
-        <f>SUM(G7:G22)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="9">
-        <f>F23-G23</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B2:I4"/>
-    <mergeCell ref="F5:H5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="143" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="143" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -962,88 +534,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="I2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
@@ -1056,7 +628,7 @@
         <v>1500000</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
@@ -1088,7 +660,7 @@
         <v>1600000</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="I8" s="2">
@@ -1123,10 +695,10 @@
         <v>1000000</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1138,10 +710,18 @@
       <c r="I10" s="2">
         <v>4</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="2:13" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>

</xml_diff>